<commit_message>
fix error in linux
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Server.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Server.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\project\NFrame_CPP\_Out\Server\NFDataCfg\Excel_Ini\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>ServerID</t>
   </si>
@@ -39,10 +44,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>127.0.0.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GameServer_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -61,9 +62,6 @@
     <t>ProxyServer_1</t>
   </si>
   <si>
-    <t>127.0.0.1</t>
-  </si>
-  <si>
     <t>MasterServer_1</t>
   </si>
   <si>
@@ -90,12 +88,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GameServer_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>192.168.1.113</t>
+  </si>
+  <si>
+    <t>192.168.1.114</t>
+  </si>
+  <si>
+    <t>192.168.1.115</t>
+  </si>
+  <si>
+    <t>192.168.1.116</t>
+  </si>
+  <si>
+    <t>192.168.1.117</t>
   </si>
 </sst>
 </file>
@@ -507,7 +512,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -517,6 +522,7 @@
     <col min="3" max="3" width="15.75" customWidth="1"/>
     <col min="4" max="4" width="11.625" customWidth="1"/>
     <col min="5" max="5" width="8.25" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.625" customWidth="1"/>
     <col min="8" max="8" width="9.375" customWidth="1"/>
   </cols>
@@ -544,18 +550,18 @@
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>5000</v>
@@ -564,24 +570,24 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G2">
         <v>16001</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
       <c r="D3">
         <v>5000</v>
@@ -590,24 +596,24 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G3">
         <v>17001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>5000</v>
@@ -616,24 +622,24 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G4">
         <v>15001</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>5000</v>
@@ -642,24 +648,24 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G5">
         <v>13001</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>5000</v>
@@ -668,40 +674,21 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G6" s="3">
         <v>14001</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>5000</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7">
-        <v>16002</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add log.conf for release remove libglog.dll
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Server.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Server.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>ServerID</t>
   </si>
@@ -88,19 +88,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>192.168.1.113</t>
-  </si>
-  <si>
-    <t>192.168.1.114</t>
-  </si>
-  <si>
-    <t>192.168.1.115</t>
-  </si>
-  <si>
-    <t>192.168.1.116</t>
-  </si>
-  <si>
-    <t>192.168.1.117</t>
+    <t>127.0.0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -512,7 +501,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -596,7 +585,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>17001</v>
@@ -622,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G4">
         <v>15001</v>
@@ -648,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G5">
         <v>13001</v>
@@ -674,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>14001</v>

</xml_diff>

<commit_message>
add area property for server
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Server.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Server.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherish\Desktop\git\nf\develop\_Out\Server\NFDataCfg\Excel_Ini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Desktop/NoahGameFrame/_Out/Server/NFDataCfg/Excel_Ini/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27520" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27740" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Id</t>
   </si>
@@ -133,12 +133,33 @@
   <si>
     <t>Upload</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameServer</t>
+  </si>
+  <si>
+    <t>WorldServer</t>
+  </si>
+  <si>
+    <t>ProxyServer</t>
+  </si>
+  <si>
+    <t>MasterServer</t>
+  </si>
+  <si>
+    <t>LoginServer</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>区服</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -365,7 +386,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
@@ -709,26 +730,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.1796875" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="22.6328125" customWidth="1"/>
-    <col min="8" max="8" width="9.36328125" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -753,8 +774,11 @@
       <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -779,34 +803,40 @@
       <c r="H2" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -831,8 +861,11 @@
       <c r="H4" s="9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
@@ -857,8 +890,11 @@
       <c r="H5" s="9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -883,8 +919,11 @@
       <c r="H6" s="9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -909,8 +948,11 @@
       <c r="H7" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
         <v>34</v>
       </c>
@@ -935,8 +977,11 @@
       <c r="H8" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="I8" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
@@ -961,8 +1006,11 @@
       <c r="H9" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
         <v>23</v>
       </c>
@@ -970,7 +1018,7 @@
         <v>24</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D10">
         <v>5000</v>
@@ -987,8 +1035,11 @@
       <c r="H10" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
         <v>26</v>
       </c>
@@ -996,7 +1047,7 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D11">
         <v>5000</v>
@@ -1013,8 +1064,11 @@
       <c r="H11" s="13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="13" t="s">
         <v>28</v>
       </c>
@@ -1022,7 +1076,7 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>5000</v>
@@ -1039,8 +1093,11 @@
       <c r="H12" s="13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="13" t="s">
         <v>30</v>
       </c>
@@ -1048,7 +1105,7 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>5000</v>
@@ -1065,8 +1122,11 @@
       <c r="H13" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
         <v>32</v>
       </c>
@@ -1074,7 +1134,7 @@
         <v>33</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D14">
         <v>5000</v>
@@ -1090,13 +1150,16 @@
       </c>
       <c r="H14" s="14" t="s">
         <v>33</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F15:F1048576 F9 F2:F6 B7:J8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F15:F1048576 F7:F9 G7:J8 F2 B7:E8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>